<commit_message>
spreadsheet: support exploded pie chart
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/pie-chart/pie-chart.xlsx
+++ b/_examples/spreadsheet/pie-chart/pie-chart.xlsx
@@ -108,6 +108,7 @@
           <c:tx>
             <c:v>Price</c:v>
           </c:tx>
+          <c:explosion val="3"/>
           <c:cat>
             <c:strRef>
               <c:f>'Sheet 1'!A2:A6</c:f>
@@ -178,86 +179,86 @@
   <x:dimension ref="A1"/>
   <x:sheetData>
     <x:row r="1">
-      <x:c t="s">
+      <x:c r="A1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c t="s">
+      <x:c r="B1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c t="s">
+      <x:c r="C1" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c t="s">
+      <x:c r="D1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
-      <x:c t="s">
+      <x:c r="A2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="B2" t="n">
         <x:v>1.23</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="C2" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c t="str">
+      <x:c r="D2" t="str">
         <x:f>C2*B2</x:f>
       </x:c>
     </x:row>
     <x:row r="3">
-      <x:c t="s">
+      <x:c r="A3" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="B3" t="n">
         <x:v>2.46</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="C3" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c t="str">
+      <x:c r="D3" t="str">
         <x:f>C3*B3</x:f>
       </x:c>
     </x:row>
     <x:row r="4">
-      <x:c t="s">
+      <x:c r="A4" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="B4" t="n">
         <x:v>3.69</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="C4" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c t="str">
+      <x:c r="D4" t="str">
         <x:f>C4*B4</x:f>
       </x:c>
     </x:row>
     <x:row r="5">
-      <x:c t="s">
+      <x:c r="A5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="B5" t="n">
         <x:v>4.92</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="C5" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c t="str">
+      <x:c r="D5" t="str">
         <x:f>C5*B5</x:f>
       </x:c>
     </x:row>
     <x:row r="6">
-      <x:c t="s">
+      <x:c r="A6" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="B6" t="n">
         <x:v>6.15</x:v>
       </x:c>
-      <x:c t="n">
+      <x:c r="C6" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c t="str">
+      <x:c r="D6" t="str">
         <x:f>C6*B6</x:f>
       </x:c>
     </x:row>

</xml_diff>